<commit_message>
may 23 4 pm update
</commit_message>
<xml_diff>
--- a/ghgtools_ActivityData.xlsx
+++ b/ghgtools_ActivityData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brand\OneDrive\Documents\GitHub\GHG-Inventory-Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6735E6E4-5768-41A2-9931-F4A282CBC50B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93D281EC-5A07-408A-9ADB-F9AA38DA6D33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="3765" yWindow="-12630" windowWidth="17250" windowHeight="8865" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16500" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ActivityData" sheetId="1" r:id="rId1"/>
@@ -964,7 +964,7 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>